<commit_message>
Procédure de test Fini
</commit_message>
<xml_diff>
--- a/procedure_de_tests_systeme.xlsx
+++ b/procedure_de_tests_systeme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camfo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\SecurityDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD44FA3C-E187-4017-937A-76D08627828F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AADFA3-E9C7-49B2-8D75-BAC21DF55450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{363E6308-B9AB-4720-BA0A-F03F882809ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t xml:space="preserve">   </t>
   </si>
@@ -36,9 +36,6 @@
     <t>Responsable:</t>
   </si>
   <si>
-    <t>Schéma Électrique</t>
-  </si>
-  <si>
     <t>Catégorie</t>
   </si>
   <si>
@@ -220,6 +217,54 @@
   </si>
   <si>
     <t>S'assurer de pouvoir lire le ADC et avoir une lecture fiable</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Test Audio</t>
+  </si>
+  <si>
+    <t>S'assurer que l'enregistrement et le speaker fonctionne</t>
+  </si>
+  <si>
+    <t>Fonctionnel</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Logiciel</t>
+  </si>
+  <si>
+    <t>S'assurer que chaque option du panneau soit fonctionnel</t>
+  </si>
+  <si>
+    <t>Option de désactivation des capteurs, changement de code etc.</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>Tester les options du panneau</t>
+  </si>
+  <si>
+    <t>Tester la communication Wifi</t>
+  </si>
+  <si>
+    <t>Communication UDP fonctionnel avec une page web basique</t>
+  </si>
+  <si>
+    <t>Avoir le serveur web fonctionnel pour se connecter avec des appareils</t>
+  </si>
+  <si>
+    <t>Liste des tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention le test pourrais endommagé la carte </t>
+  </si>
+  <si>
+    <t>Afficher les trois couleur sur chaque pixel</t>
   </si>
 </sst>
 </file>
@@ -299,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,10 +366,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB617CFD-806A-4BDF-9158-25E8F0AEA573}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -718,7 +760,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.85">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -752,7 +794,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -766,51 +808,51 @@
     </row>
     <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.65">
       <c r="A13" s="4" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="F14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -818,39 +860,41 @@
     </row>
     <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -858,19 +902,19 @@
     </row>
     <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -878,19 +922,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -898,19 +942,19 @@
     </row>
     <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -918,19 +962,19 @@
     </row>
     <row r="21" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -938,39 +982,41 @@
     </row>
     <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="H22" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -978,16 +1024,16 @@
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -996,73 +1042,107 @@
     </row>
     <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="A28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.9</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+      <c r="H28" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="7"/>

</xml_diff>